<commit_message>
Components added to BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>S.No.</t>
   </si>
@@ -66,12 +66,6 @@
     <t>https://goo.gl/LD6cmX</t>
   </si>
   <si>
-    <t>Bread board with cables</t>
-  </si>
-  <si>
-    <t>https://goo.gl/64hoQJ</t>
-  </si>
-  <si>
     <t>Multimeter</t>
   </si>
   <si>
@@ -96,10 +90,46 @@
     <t>COMPONENT</t>
   </si>
   <si>
-    <t>7.4V 3500 mAh 35C LiPo battery</t>
-  </si>
-  <si>
-    <t>https://goo.gl/nKJf7g</t>
+    <t>Bread board with Power module and jumper cables</t>
+  </si>
+  <si>
+    <t>https://goo.gl/GiHjuM</t>
+  </si>
+  <si>
+    <t>7.4V 1500 mAh 25C LiPo battery for motors</t>
+  </si>
+  <si>
+    <t>https://goo.gl/PEDWJU</t>
+  </si>
+  <si>
+    <t>5v 2.4 A Power bank for Raspberry Pi</t>
+  </si>
+  <si>
+    <t>https://goo.gl/o323cW</t>
+  </si>
+  <si>
+    <t>9V 1A AC-DC Converter for Breadboard</t>
+  </si>
+  <si>
+    <t>https://goo.gl/Jt5Dpn</t>
+  </si>
+  <si>
+    <t>Double sided foam tape</t>
+  </si>
+  <si>
+    <t>https://goo.gl/7ENrhd</t>
+  </si>
+  <si>
+    <t>Anti Static ESD Gloves</t>
+  </si>
+  <si>
+    <t>https://goo.gl/7yG2hZ</t>
+  </si>
+  <si>
+    <t>Raspberry Pi base plate Holder</t>
+  </si>
+  <si>
+    <t>https://goo.gl/eMxNbV</t>
   </si>
 </sst>
 </file>
@@ -472,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,16 +520,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -538,9 +568,9 @@
         <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -605,13 +635,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -619,13 +649,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,7 +668,7 @@
       <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -647,21 +677,95 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{6B8E0675-BF44-451E-9F2F-386E48BB564D}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{FCEE539A-F358-4542-AE5D-07582746D0AB}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{2C4FE278-69D8-44E1-B5B4-9E9B032E1361}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{B250086B-B21A-4DD5-8180-697E969670EB}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{EC16B7BB-42E0-40D1-AA1C-00AFE2BF1BEB}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{6922ABC6-8D59-4B98-A983-9D382AB9D000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{13D3452E-D2DC-4571-91E1-4FBF642B1BF2}"/>
+    <hyperlink ref="D15" r:id="rId6" xr:uid="{C947D67E-686F-41F9-96B4-ACBD431E82D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>